<commit_message>
Correct some bugs; add some error detection; update README
</commit_message>
<xml_diff>
--- a/examples/basic/basic.xlsx
+++ b/examples/basic/basic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisnar/matlab/OLMOODLE/examples/basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460A4824-FEF8-4A4E-A2E2-D56E9E47E23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B4D15E-56EE-C145-8613-78CF7233C470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="4400" windowWidth="23600" windowHeight="16320" xr2:uid="{58FCA027-E9DA-F143-BE25-1E531D79B372}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,9 +54,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Formattage</t>
-  </si>
-  <si>
     <t>Vous avez droit à une marge d'erreur relative de</t>
   </si>
   <si>
@@ -144,6 +142,9 @@
   </si>
   <si>
     <t>Q*</t>
+  </si>
+  <si>
+    <t>Format</t>
   </si>
 </sst>
 </file>
@@ -706,7 +707,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -724,10 +725,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -735,10 +736,10 @@
     </row>
     <row r="2" spans="1:9" ht="17">
       <c r="A2" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -746,7 +747,7 @@
     </row>
     <row r="3" spans="1:9" ht="17">
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -754,7 +755,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="5">
         <v>10</v>
@@ -774,13 +775,13 @@
     </row>
     <row r="6" spans="1:9" ht="32" customHeight="1">
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>3</v>
@@ -789,13 +790,13 @@
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="32" customHeight="1">
@@ -803,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
@@ -814,13 +815,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="18">
         <v>10</v>
@@ -833,7 +834,7 @@
       </c>
       <c r="H8" s="18"/>
       <c r="I8" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17">
@@ -841,13 +842,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" s="18">
         <v>10</v>
@@ -860,7 +861,7 @@
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -876,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="26"/>
       <c r="I11" s="2"/>
@@ -887,7 +888,7 @@
       <c r="C12" s="26"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -896,73 +897,73 @@
     </row>
     <row r="13" spans="1:9" ht="17">
       <c r="A13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="10"/>
       <c r="I13" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17">
       <c r="A14" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="10"/>
       <c r="I14" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17">
       <c r="A15" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="10"/>
       <c r="I15" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="22" customHeight="1">
       <c r="A16" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="17"/>
@@ -973,7 +974,7 @@
         <v>2</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>